<commit_message>
Updates Clava Restructuring Excel
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="210">
   <si>
     <t>Node</t>
   </si>
@@ -652,6 +652,9 @@
   </si>
   <si>
     <t>Pragma</t>
+  </si>
+  <si>
+    <t>ClavaNode</t>
   </si>
 </sst>
 </file>
@@ -1111,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,7 +1129,7 @@
       </c>
       <c r="B2">
         <f>SUM(decl!D2,expr!D2,stmt!D2,type!D2,attr!D2,other!D2)</f>
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1135,7 +1138,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1144,7 +1147,7 @@
       </c>
       <c r="B4">
         <f>SUM(decl!F2,expr!F2,stmt!F2,type!F2,attr!F2,other!F2)</f>
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1152,8 +1155,8 @@
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <f>B3/B2</f>
-        <v>5.0000000000000001E-3</v>
+        <f>(B3 + (B4/2))/B2</f>
+        <v>9.4527363184079602E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1166,7 +1169,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,9 +1199,6 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
         <v>38</v>
@@ -1216,9 +1216,6 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1249,6 +1246,9 @@
       <c r="A9" t="s">
         <v>16</v>
       </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1258,6 +1258,9 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1439,7 +1442,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A62"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,11 +1478,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1501,11 +1504,17 @@
       <c r="A6" t="s">
         <v>51</v>
       </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1531,6 +1540,9 @@
       <c r="A12" t="s">
         <v>57</v>
       </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1632,82 +1644,103 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -1821,7 +1854,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A27"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,7 +1894,7 @@
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1923,68 +1956,77 @@
       <c r="A14" t="s">
         <v>120</v>
       </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>133</v>
       </c>
@@ -2027,8 +2069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,11 +2106,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2090,6 +2132,9 @@
       <c r="A6" t="s">
         <v>138</v>
       </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2115,6 +2160,9 @@
       <c r="A11" t="s">
         <v>143</v>
       </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2140,113 +2188,128 @@
       <c r="A16" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>170</v>
       </c>
@@ -2290,7 +2353,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,37 +2383,52 @@
       <c r="A2" t="s">
         <v>171</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
         <v>9</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>172</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>173</v>
       </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>174</v>
       </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>175</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2409,10 +2487,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2440,158 +2518,169 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>209</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>190</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>208</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[ClavaWeaver] Replaces uses of ClavaNodesLegacy
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="210">
   <si>
     <t>Node</t>
   </si>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="B4">
         <f>SUM(decl!F2,expr!F2,stmt!F2,type!F2,attr!F2,other!F2)</f>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.10199004975124377</v>
+        <v>0.11691542288557213</v>
       </c>
     </row>
   </sheetData>
@@ -1441,7 +1441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
@@ -1856,7 +1856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1893,11 +1893,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1968,7 +1968,7 @@
         <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2072,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,11 +2109,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2181,18 +2181,24 @@
       <c r="A14" t="s">
         <v>146</v>
       </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>147</v>
       </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates Excel file with node migration status
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="210">
   <si>
     <t>Node</t>
   </si>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.12686567164179105</v>
+        <v>0.13681592039800994</v>
       </c>
     </row>
   </sheetData>
@@ -1857,7 +1857,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1919,6 +1919,9 @@
       <c r="A6" t="s">
         <v>112</v>
       </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1992,6 +1995,9 @@
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates Excel with restructuring progress
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="214">
   <si>
     <t>Node</t>
   </si>
@@ -655,6 +655,18 @@
   </si>
   <si>
     <t>ClavaNode</t>
+  </si>
+  <si>
+    <t>CompoundLiteralExpr</t>
+  </si>
+  <si>
+    <t>Needs Clean</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>clean</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1129,7 +1141,7 @@
       </c>
       <c r="B2">
         <f>SUM(decl!D2,expr!D2,stmt!D2,type!D2,attr!D2,other!D2)</f>
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1138,7 +1150,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1156,7 +1168,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.13681592039800994</v>
+        <v>0.1707920792079208</v>
       </c>
     </row>
   </sheetData>
@@ -1169,7 +1181,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,11 +1217,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1247,7 +1259,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1439,15 +1451,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1458,6 +1471,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1474,15 +1490,15 @@
       </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1523,298 +1539,318 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>210</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>79</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>81</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>83</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>85</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C41" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>88</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>90</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>91</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1856,7 +1892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2085,7 +2121,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,7 +2157,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -2132,6 +2168,12 @@
       <c r="A3" t="s">
         <v>135</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2155,6 +2197,12 @@
       <c r="A7" t="s">
         <v>139</v>
       </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2213,17 +2261,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>151</v>
       </c>
@@ -2231,12 +2285,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>153</v>
       </c>
@@ -2244,22 +2298,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -2267,42 +2321,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -2310,29 +2364,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>170</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates status of Clava Parser restructuring
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="224">
   <si>
     <t>Node</t>
   </si>
@@ -688,6 +688,15 @@
   </si>
   <si>
     <t>UnresolvedUsingValueDecl</t>
+  </si>
+  <si>
+    <t>UnusedAttr</t>
+  </si>
+  <si>
+    <t>TypeAliasTemplateDecl</t>
+  </si>
+  <si>
+    <t>NonTypeTemplateParmDecl</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1157,7 @@
   <dimension ref="A2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1171,7 @@
       </c>
       <c r="B2">
         <f>SUM(decl!D2,expr!D2,stmt!D2,type!D2,attr!D2,other!D2)</f>
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1171,7 +1180,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>65</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1180,7 +1189,7 @@
       </c>
       <c r="B4">
         <f>SUM(decl!F2,expr!F2,stmt!F2,type!F2,attr!F2,other!F2)</f>
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1189,7 +1198,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.36124401913875598</v>
+        <v>0.44811320754716982</v>
       </c>
     </row>
   </sheetData>
@@ -1199,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,21 +1243,24 @@
       </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1326,7 +1338,7 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,6 +1353,9 @@
       <c r="A13" t="s">
         <v>19</v>
       </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1354,6 +1369,9 @@
       <c r="A15" t="s">
         <v>21</v>
       </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1372,6 +1390,9 @@
       <c r="A18" t="s">
         <v>24</v>
       </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1413,39 +1434,42 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>223</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
         <v>2</v>
@@ -1453,63 +1477,69 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>222</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>220</v>
-      </c>
-      <c r="B39" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>220</v>
       </c>
       <c r="B41" t="s">
         <v>2</v>
@@ -1517,7 +1547,26 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1558,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,11 +1648,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1615,6 +1664,9 @@
       <c r="A4" t="s">
         <v>49</v>
       </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1641,6 +1693,9 @@
       <c r="A8" t="s">
         <v>53</v>
       </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1693,6 +1748,9 @@
       <c r="A16" t="s">
         <v>60</v>
       </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1713,6 +1771,9 @@
       <c r="A20" t="s">
         <v>64</v>
       </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1845,7 +1906,7 @@
         <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
         <v>212</v>
@@ -1939,6 +2000,9 @@
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>97</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2271,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2302,13 +2366,16 @@
       <c r="A2" t="s">
         <v>134</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
         <v>38</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -2358,6 +2425,9 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>140</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2638,10 +2708,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,11 +2749,11 @@
       </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -2754,6 +2824,14 @@
       </c>
       <c r="C11" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converts all CastExpr nodes to the new format
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="227">
   <si>
     <t>Node</t>
   </si>
@@ -558,9 +558,6 @@
     <t>FinalAttr</t>
   </si>
   <si>
-    <t>GenericAttribute</t>
-  </si>
-  <si>
     <t>InheritableAttr</t>
   </si>
   <si>
@@ -624,9 +621,6 @@
     <t>Undefined</t>
   </si>
   <si>
-    <t>VariadicType</t>
-  </si>
-  <si>
     <t>OmpClausePragma</t>
   </si>
   <si>
@@ -697,6 +691,21 @@
   </si>
   <si>
     <t>NonTypeTemplateParmDecl</t>
+  </si>
+  <si>
+    <t>TypeVisibilityAttr</t>
+  </si>
+  <si>
+    <t>MaxFieldalignmentAttr</t>
+  </si>
+  <si>
+    <t>NoThrowAttr</t>
+  </si>
+  <si>
+    <t>RestrictAttr</t>
+  </si>
+  <si>
+    <t>PureAttr</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
@@ -1171,7 +1180,7 @@
       </c>
       <c r="B2">
         <f>SUM(decl!D2,expr!D2,stmt!D2,type!D2,attr!D2,other!D2)</f>
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1180,7 +1189,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>86</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1189,7 +1198,7 @@
       </c>
       <c r="B4">
         <f>SUM(decl!F2,expr!F2,stmt!F2,type!F2,attr!F2,other!F2)</f>
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1198,7 +1207,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.44811320754716982</v>
+        <v>0.61860465116279073</v>
       </c>
     </row>
   </sheetData>
@@ -1210,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,13 +1250,16 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
         <v>43</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1264,7 +1276,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1278,7 +1290,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1289,7 +1301,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1300,7 +1312,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1311,7 +1323,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1322,7 +1334,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1401,7 +1413,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
@@ -1434,7 +1446,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
@@ -1464,7 +1476,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1503,10 +1515,13 @@
       <c r="A34" t="s">
         <v>38</v>
       </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -1516,16 +1531,25 @@
       <c r="A36" t="s">
         <v>39</v>
       </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1539,7 +1563,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B41" t="s">
         <v>2</v>
@@ -1607,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1650,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1648,11 +1672,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1699,7 +1723,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -1714,6 +1738,9 @@
       <c r="A11" t="s">
         <v>55</v>
       </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1735,6 +1762,9 @@
       <c r="A14" t="s">
         <v>58</v>
       </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1787,6 +1817,9 @@
       <c r="A22" t="s">
         <v>66</v>
       </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1797,6 +1830,9 @@
       <c r="A24" t="s">
         <v>68</v>
       </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1810,11 +1846,17 @@
       <c r="A26" t="s">
         <v>70</v>
       </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>71</v>
       </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1840,6 +1882,9 @@
       <c r="A32" t="s">
         <v>76</v>
       </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1856,7 +1901,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -1874,6 +1919,9 @@
       <c r="A37" t="s">
         <v>80</v>
       </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1887,6 +1935,9 @@
       <c r="A39" t="s">
         <v>82</v>
       </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1909,7 +1960,7 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1920,7 +1971,7 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1994,7 +2045,7 @@
         <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2049,10 +2100,13 @@
       <c r="A63" t="s">
         <v>106</v>
       </c>
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B64" t="s">
         <v>2</v>
@@ -2336,7 +2390,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,11 +2429,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2390,25 +2444,31 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>136</v>
       </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>137</v>
       </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>138</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2419,7 +2479,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2434,26 +2494,32 @@
       <c r="A9" t="s">
         <v>141</v>
       </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>142</v>
       </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2464,7 +2530,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2475,7 +2541,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2510,13 +2576,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>150</v>
       </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2530,6 +2599,9 @@
       <c r="A21" t="s">
         <v>152</v>
       </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2543,11 +2615,17 @@
       <c r="A23" t="s">
         <v>154</v>
       </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>155</v>
       </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2557,7 +2635,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2576,23 +2654,32 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>159</v>
       </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>160</v>
       </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>161</v>
       </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -2602,7 +2689,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2621,7 +2708,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2629,7 +2716,7 @@
         <v>165</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2644,6 +2731,9 @@
       <c r="A36" t="s">
         <v>167</v>
       </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2653,13 +2743,16 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>169</v>
       </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -2669,7 +2762,7 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2708,10 +2801,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2749,15 +2842,15 @@
       </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2781,12 +2874,12 @@
         <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -2804,33 +2897,74 @@
       <c r="A8" t="s">
         <v>176</v>
       </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>177</v>
       </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>178</v>
+        <v>223</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2870,10 +3004,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2901,14 +3035,14 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
@@ -2921,57 +3055,57 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -2979,7 +3113,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -2987,93 +3121,88 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converts node 'CXXDependentScopeMemberExpr' to new format
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="227">
   <si>
     <t>Node</t>
   </si>
@@ -1165,7 +1165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1207,7 +1207,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.61860465116279073</v>
+        <v>0.62325581395348839</v>
       </c>
     </row>
   </sheetData>
@@ -1631,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1795,6 +1795,9 @@
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converts IfStmt, adds ChildrenAdapter and renames NullNode to NullNodeOld
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="227">
   <si>
     <t>Node</t>
   </si>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1207,7 +1207,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.62325581395348839</v>
+        <v>0.62790697674418605</v>
       </c>
     </row>
   </sheetData>
@@ -1632,7 +1632,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1874,6 +1874,9 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converts several nodes to the new format
- ArraySubscriptExpr, ParenExpr, ParenListExpr;
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="228">
   <si>
     <t>Node</t>
   </si>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.64351851851851849</v>
+        <v>0.65740740740740744</v>
       </c>
     </row>
   </sheetData>
@@ -1634,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1686,6 +1686,9 @@
       <c r="A3" t="s">
         <v>48</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2077,10 +2080,16 @@
       <c r="A56" t="s">
         <v>98</v>
       </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>99</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converts WhileStmt to new format
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="228">
   <si>
     <t>Node</t>
   </si>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B4">
         <f>SUM(decl!F2,expr!F2,stmt!F2,type!F2,attr!F2,other!F2)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.65740740740740744</v>
+        <v>0.66898148148148151</v>
       </c>
     </row>
   </sheetData>
@@ -1634,7 +1634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
@@ -2190,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2227,11 +2227,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2315,6 +2315,9 @@
       <c r="A16" t="s">
         <v>122</v>
       </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2341,6 +2344,9 @@
       <c r="A20" t="s">
         <v>126</v>
       </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2379,6 +2385,9 @@
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>132</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converts CXXForRangeStmt, ContinueStmt and BreakStmt
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="228">
   <si>
     <t>Node</t>
   </si>
@@ -1168,7 +1168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B4">
         <f>SUM(decl!F2,expr!F2,stmt!F2,type!F2,attr!F2,other!F2)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.66898148148148151</v>
+        <v>0.68981481481481477</v>
       </c>
     </row>
   </sheetData>
@@ -2190,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,17 +2221,20 @@
       <c r="A2" t="s">
         <v>108</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
         <v>26</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2261,6 +2264,9 @@
       <c r="A7" t="s">
         <v>113</v>
       </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2271,6 +2277,9 @@
       <c r="A9" t="s">
         <v>115</v>
       </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2294,6 +2303,9 @@
       <c r="A13" t="s">
         <v>119</v>
       </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2345,7 +2357,7 @@
         <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converts nodes NamespaceDecl, UsingDecl, UsingDirectiveDecl and CXXUnresolvedConstructExpr
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="228">
   <si>
     <t>Node</t>
   </si>
@@ -1168,7 +1168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.68981481481481477</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
   </sheetData>
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1446,6 +1446,9 @@
       <c r="A25" t="s">
         <v>30</v>
       </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1558,10 +1561,16 @@
       <c r="A39" t="s">
         <v>42</v>
       </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1635,7 +1644,7 @@
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1684,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1901,6 +1910,9 @@
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converts node CXXCatchStmt and removes all legacy Literal nodes
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B4">
         <f>SUM(decl!F2,expr!F2,stmt!F2,type!F2,attr!F2,other!F2)</f>
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.72685185185185186</v>
+        <v>0.73842592592592593</v>
       </c>
     </row>
   </sheetData>
@@ -1643,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,11 +1687,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1728,7 +1728,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1744,7 +1744,7 @@
         <v>208</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1948,7 +1948,7 @@
         <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1980,7 +1980,7 @@
         <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2023,7 +2023,7 @@
         <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converts node FriendDecl, adds C++ test 'friend'
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="228">
   <si>
     <t>Node</t>
   </si>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B4">
         <f>SUM(decl!F2,expr!F2,stmt!F2,type!F2,attr!F2,other!F2)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.73842592592592593</v>
+        <v>0.76388888888888884</v>
       </c>
     </row>
   </sheetData>
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1391,6 +1391,9 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1643,8 +1646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,11 +1690,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1910,6 +1913,9 @@
       <c r="A31" t="s">
         <v>75</v>
       </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2036,7 +2042,7 @@
         <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2134,6 +2140,9 @@
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>103</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2215,7 +2224,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,7 +2263,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -2296,6 +2305,9 @@
       <c r="A8" t="s">
         <v>114</v>
       </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2308,6 +2320,9 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>116</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converted nodes OffsetOfExpr, GNUNullExpr and StmtExpr
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="228">
   <si>
     <t>Node</t>
   </si>
@@ -1168,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.76851851851851849</v>
+        <v>0.78240740740740744</v>
       </c>
     </row>
   </sheetData>
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1996,6 +1996,9 @@
       <c r="A41" t="s">
         <v>84</v>
       </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -2084,6 +2087,9 @@
       <c r="A52" t="s">
         <v>95</v>
       </c>
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -2138,6 +2144,9 @@
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>102</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converts nodes CXXStdInitializerListExpr and LiteralDecl
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="228">
   <si>
     <t>Node</t>
   </si>
@@ -1168,7 +1168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.78240740740740744</v>
+        <v>0.79629629629629628</v>
       </c>
     </row>
   </sheetData>
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1436,6 +1436,9 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1649,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,7 +1696,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1898,10 +1901,16 @@
       <c r="A28" t="s">
         <v>72</v>
       </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converts nodes NamespaceAliasDecl and NullDecl
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="228">
   <si>
     <t>Node</t>
   </si>
@@ -1168,7 +1168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B3">
         <f>SUM(decl!E2,expr!E2,stmt!E2,type!E2,attr!E2,other!E2)</f>
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B4">
         <f>SUM(decl!F2,expr!F2,stmt!F2,type!F2,attr!F2,other!F2)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.79629629629629628</v>
+        <v>0.80787037037037035</v>
       </c>
     </row>
   </sheetData>
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,11 +1262,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1445,11 +1445,17 @@
       <c r="A23" t="s">
         <v>28</v>
       </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1472,7 +1478,7 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converts nodes SwitchStmt, CaseStmt and DefaultStmt
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
     <sheet name="-decl-" sheetId="1" r:id="rId2"/>
-    <sheet name="expr" sheetId="4" r:id="rId3"/>
+    <sheet name="-expr-" sheetId="4" r:id="rId3"/>
     <sheet name="stmt" sheetId="5" r:id="rId4"/>
     <sheet name="-type-" sheetId="7" r:id="rId5"/>
     <sheet name="-attr-" sheetId="8" r:id="rId6"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="228">
   <si>
     <t>Node</t>
   </si>
@@ -1182,7 +1182,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <f>SUM('-decl-'!D2,expr!D2,stmt!D2,'-type-'!D2,'-attr-'!D2,other!D2)</f>
+        <f>SUM('-decl-'!D2,'-expr-'!D2,stmt!D2,'-type-'!D2,'-attr-'!D2,other!D2)</f>
         <v>216</v>
       </c>
     </row>
@@ -1191,8 +1191,8 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <f>SUM('-decl-'!E2,expr!E2,stmt!E2,'-type-'!E2,'-attr-'!E2,other!E2)</f>
-        <v>180</v>
+        <f>SUM('-decl-'!E2,'-expr-'!E2,stmt!E2,'-type-'!E2,'-attr-'!E2,other!E2)</f>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1200,7 +1200,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <f>SUM('-decl-'!F2,expr!F2,stmt!F2,'-type-'!F2,'-attr-'!F2,other!F2)</f>
+        <f>SUM('-decl-'!F2,'-expr-'!F2,stmt!F2,'-type-'!F2,'-attr-'!F2,other!F2)</f>
         <v>5</v>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.84490740740740744</v>
+        <v>0.86805555555555558</v>
       </c>
     </row>
   </sheetData>
@@ -1661,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -2169,6 +2169,9 @@
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>101</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2265,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,7 +2308,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -2321,6 +2324,9 @@
       <c r="A4" t="s">
         <v>110</v>
       </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2379,6 +2385,9 @@
       <c r="A12" t="s">
         <v>118</v>
       </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2469,10 +2478,16 @@
       <c r="A24" t="s">
         <v>130</v>
       </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adds nodes LabelDecl and GotoStmt, converts LabelStmt and WrapperStmt
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="230">
   <si>
     <t>Node</t>
   </si>
@@ -709,6 +709,12 @@
   </si>
   <si>
     <t>OpaqueValueExpr</t>
+  </si>
+  <si>
+    <t>GotoStmt</t>
+  </si>
+  <si>
+    <t>LabelDecl</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1189,7 @@
       </c>
       <c r="B2">
         <f>SUM('-decl-'!D2,'-expr-'!D2,stmt!D2,'-type-'!D2,'-attr-'!D2,other!D2)</f>
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1192,7 +1198,7 @@
       </c>
       <c r="B3">
         <f>SUM('-decl-'!E2,'-expr-'!E2,stmt!E2,'-type-'!E2,'-attr-'!E2,other!E2)</f>
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1216,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.86805555555555558</v>
+        <v>0.87844036697247707</v>
       </c>
     </row>
   </sheetData>
@@ -1220,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,11 +1264,11 @@
       </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -1430,7 +1436,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>229</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
@@ -1438,7 +1444,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
@@ -1446,7 +1452,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
@@ -1454,7 +1460,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
@@ -1462,7 +1468,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
@@ -1470,7 +1476,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>221</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
@@ -1478,7 +1484,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>221</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
@@ -1486,7 +1492,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
@@ -1494,26 +1500,26 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
         <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
         <v>2</v>
@@ -1521,7 +1527,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>2</v>
@@ -1529,7 +1535,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
@@ -1537,7 +1543,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>2</v>
@@ -1545,7 +1551,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>220</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -1553,7 +1559,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>220</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -1561,7 +1567,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
         <v>2</v>
@@ -1569,7 +1575,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
@@ -1577,7 +1583,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -1585,7 +1591,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
         <v>2</v>
@@ -1593,7 +1599,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>218</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
         <v>2</v>
@@ -1601,7 +1607,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>218</v>
       </c>
       <c r="B42" t="s">
         <v>2</v>
@@ -1609,7 +1615,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
         <v>2</v>
@@ -1617,9 +1623,17 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>46</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1661,7 +1675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -2266,10 +2280,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,11 +2318,11 @@
       </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
@@ -2423,7 +2437,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>228</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -2431,12 +2445,15 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -2444,7 +2461,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
@@ -2452,39 +2469,39 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
@@ -2492,7 +2509,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
@@ -2500,7 +2517,18 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>133</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converts all Stmt nodes, all nodes that depend of dumper are now converted
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8850" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
     <sheet name="-decl-" sheetId="1" r:id="rId2"/>
     <sheet name="-expr-" sheetId="4" r:id="rId3"/>
-    <sheet name="stmt" sheetId="5" r:id="rId4"/>
+    <sheet name="-stmt-" sheetId="5" r:id="rId4"/>
     <sheet name="-type-" sheetId="7" r:id="rId5"/>
     <sheet name="-attr-" sheetId="8" r:id="rId6"/>
     <sheet name="other" sheetId="9" r:id="rId7"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="229">
   <si>
     <t>Node</t>
   </si>
@@ -358,9 +358,6 @@
   </si>
   <si>
     <t>CaseStmt</t>
-  </si>
-  <si>
-    <t>ClangLabelStmt</t>
   </si>
   <si>
     <t>CompoundStmt</t>
@@ -1188,8 +1185,8 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <f>SUM('-decl-'!D2,'-expr-'!D2,stmt!D2,'-type-'!D2,'-attr-'!D2,other!D2)</f>
-        <v>218</v>
+        <f>SUM('-decl-'!D2,'-expr-'!D2,'-stmt-'!D2,'-type-'!D2,'-attr-'!D2,other!D2)</f>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1197,8 +1194,8 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <f>SUM('-decl-'!E2,'-expr-'!E2,stmt!E2,'-type-'!E2,'-attr-'!E2,other!E2)</f>
-        <v>189</v>
+        <f>SUM('-decl-'!E2,'-expr-'!E2,'-stmt-'!E2,'-type-'!E2,'-attr-'!E2,other!E2)</f>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1206,8 +1203,8 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <f>SUM('-decl-'!F2,'-expr-'!F2,stmt!F2,'-type-'!F2,'-attr-'!F2,other!F2)</f>
-        <v>5</v>
+        <f>SUM('-decl-'!F2,'-expr-'!F2,'-stmt-'!F2,'-type-'!F2,'-attr-'!F2,other!F2)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1216,7 +1213,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.87844036697247707</v>
+        <v>0.89400921658986177</v>
       </c>
     </row>
   </sheetData>
@@ -1285,7 +1282,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1299,7 +1296,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1310,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1321,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1332,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1343,7 +1340,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1428,7 +1425,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
@@ -1436,7 +1433,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
@@ -1484,7 +1481,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
@@ -1514,7 +1511,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1559,7 +1556,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -1607,7 +1604,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B42" t="s">
         <v>2</v>
@@ -1694,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1776,7 +1773,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -1984,7 +1981,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -2046,7 +2043,7 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2057,7 +2054,7 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2134,7 +2131,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B53" t="s">
         <v>2</v>
@@ -2230,7 +2227,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B65" t="s">
         <v>2</v>
@@ -2280,10 +2277,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,21 +2315,24 @@
       </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>109</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2346,6 +2346,9 @@
       <c r="A5" t="s">
         <v>111</v>
       </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2416,7 +2419,7 @@
         <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2429,7 +2432,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>227</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -2437,7 +2440,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>228</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -2480,7 +2483,7 @@
         <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2496,7 +2499,7 @@
         <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2520,14 +2523,6 @@
         <v>132</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B28" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2598,7 +2593,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -2618,18 +2613,18 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -2637,7 +2632,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -2645,7 +2640,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -2653,18 +2648,18 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -2672,7 +2667,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -2680,7 +2675,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -2688,7 +2683,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -2696,7 +2691,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -2704,29 +2699,29 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -2734,7 +2729,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -2742,7 +2737,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -2750,18 +2745,18 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -2769,7 +2764,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
@@ -2777,7 +2772,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
@@ -2785,7 +2780,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
@@ -2793,7 +2788,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
@@ -2801,7 +2796,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
@@ -2809,18 +2804,18 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
@@ -2828,18 +2823,18 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
@@ -2847,7 +2842,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
@@ -2855,7 +2850,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B30" t="s">
         <v>2</v>
@@ -2863,18 +2858,18 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B31" t="s">
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B32" t="s">
         <v>2</v>
@@ -2882,18 +2877,18 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B34" t="s">
         <v>2</v>
@@ -2901,7 +2896,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -2909,7 +2904,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -2917,18 +2912,18 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B37" t="s">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
@@ -2936,13 +2931,13 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3001,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3015,7 +3010,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -3035,7 +3030,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -3043,7 +3038,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -3051,7 +3046,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -3059,7 +3054,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -3067,7 +3062,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -3075,7 +3070,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -3083,7 +3078,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -3091,7 +3086,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -3099,7 +3094,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -3107,18 +3102,18 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -3126,7 +3121,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -3134,7 +3129,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -3142,7 +3137,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -3186,7 +3181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -3215,7 +3210,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -3235,57 +3230,57 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -3293,7 +3288,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -3301,17 +3296,17 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -3319,7 +3314,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
@@ -3327,7 +3322,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -3335,63 +3330,63 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converts node GenericPragma to new format
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="229">
   <si>
     <t>Node</t>
   </si>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="B3">
         <f>SUM('-decl-'!E2,'-expr-'!E2,'-stmt-'!E2,'-type-'!E2,'-attr-'!E2,other!E2)</f>
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="B4">
         <f>SUM('-decl-'!F2,'-expr-'!F2,'-stmt-'!F2,'-type-'!F2,'-attr-'!F2,other!F2)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.89400921658986177</v>
+        <v>0.90092165898617516</v>
       </c>
     </row>
   </sheetData>
@@ -3181,8 +3181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3221,11 +3221,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3383,10 +3383,16 @@
       <c r="A29" t="s">
         <v>204</v>
       </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>205</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finishes conversion of nodes to new format
</commit_message>
<xml_diff>
--- a/Clava Parser Restructuring.xlsx
+++ b/Clava Parser Restructuring.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="217">
   <si>
     <t>Node</t>
   </si>
@@ -561,45 +561,24 @@
     <t>OpenCLKernelAttr</t>
   </si>
   <si>
-    <t>BlockContentComment</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
     <t>DummyComment</t>
   </si>
   <si>
-    <t>FullComment</t>
-  </si>
-  <si>
-    <t>InlineCommandComment</t>
-  </si>
-  <si>
     <t>InlineComment</t>
   </si>
   <si>
-    <t>InlineContentComment</t>
-  </si>
-  <si>
     <t>MultiLineComment</t>
   </si>
   <si>
-    <t>ParagraphComment</t>
-  </si>
-  <si>
-    <t>TextComment</t>
-  </si>
-  <si>
     <t>App</t>
   </si>
   <si>
     <t>CXXCtorInitializer</t>
   </si>
   <si>
-    <t>OriginalNamespace</t>
-  </si>
-  <si>
     <t>TemplateArgument</t>
   </si>
   <si>
@@ -612,24 +591,12 @@
     <t>TranslationUnit</t>
   </si>
   <si>
-    <t>Undefined</t>
-  </si>
-  <si>
     <t>OmpClausePragma</t>
   </si>
   <si>
-    <t>OmpDirectiveKind</t>
-  </si>
-  <si>
-    <t>OMPExecutableDirective</t>
-  </si>
-  <si>
     <t>OmpLiteralPragma</t>
   </si>
   <si>
-    <t>OMPParallelDirective</t>
-  </si>
-  <si>
     <t>OmpPragma</t>
   </si>
   <si>
@@ -709,9 +676,6 @@
   </si>
   <si>
     <t>LabelDecl</t>
-  </si>
-  <si>
-    <t>NullNodeOld</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1150,7 @@
       </c>
       <c r="B2">
         <f>SUM('-decl-'!D2,'-expr-'!D2,'-stmt-'!D2,'-type-'!D2,'-attr-'!D2,other!D2)</f>
-        <v>217</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1195,7 +1159,7 @@
       </c>
       <c r="B3">
         <f>SUM('-decl-'!E2,'-expr-'!E2,'-stmt-'!E2,'-type-'!E2,'-attr-'!E2,other!E2)</f>
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,7 +1168,7 @@
       </c>
       <c r="B4">
         <f>SUM('-decl-'!F2,'-expr-'!F2,'-stmt-'!F2,'-type-'!F2,'-attr-'!F2,other!F2)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1213,7 +1177,7 @@
       </c>
       <c r="B6" s="2">
         <f>(B3 + (B4/2))/B2</f>
-        <v>0.92165898617511521</v>
+        <v>0.99268292682926829</v>
       </c>
     </row>
   </sheetData>
@@ -1282,7 +1246,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1296,7 +1260,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1307,7 +1271,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1318,7 +1282,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1329,7 +1293,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1340,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1425,7 +1389,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
@@ -1433,7 +1397,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
@@ -1481,7 +1445,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
@@ -1511,7 +1475,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1556,7 +1520,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -1604,7 +1568,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="B42" t="s">
         <v>2</v>
@@ -1691,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1773,7 +1737,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -1981,7 +1945,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -2043,7 +2007,7 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2054,7 +2018,7 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2131,7 +2095,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B53" t="s">
         <v>2</v>
@@ -2227,7 +2191,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B65" t="s">
         <v>2</v>
@@ -2432,7 +2396,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -2619,7 +2583,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2654,7 +2618,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2675,7 +2639,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -2705,7 +2669,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2716,7 +2680,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2751,7 +2715,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2810,7 +2774,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2829,7 +2793,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2864,7 +2828,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2883,7 +2847,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2918,7 +2882,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2937,7 +2901,7 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2996,7 +2960,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3054,7 +3018,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -3086,7 +3050,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -3094,7 +3058,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -3108,12 +3072,12 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -3121,7 +3085,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -3129,7 +3093,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -3137,7 +3101,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -3179,10 +3143,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3210,73 +3174,106 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="D2">
         <f>COUNTIF(A:A, "*")-1</f>
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <f>COUNTIF(B:B, "o")</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <f>COUNTIF(B:B, "-")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>178</v>
       </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>179</v>
       </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>180</v>
       </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>181</v>
       </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>182</v>
       </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>183</v>
       </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>184</v>
       </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>185</v>
       </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>186</v>
       </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>187</v>
       </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3296,114 +3293,33 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>228</v>
+        <v>190</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>193</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>194</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>196</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>199</v>
-      </c>
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>201</v>
-      </c>
-      <c r="B27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>202</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>203</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>204</v>
-      </c>
-      <c r="B30" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>